<commit_message>
fix in progress go back and scrape data
</commit_message>
<xml_diff>
--- a/scraped_profiles.xlsx
+++ b/scraped_profiles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -22,7 +22,64 @@
     <t>University</t>
   </si>
   <si>
+    <t>Acceptance Rate</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Degree Type</t>
+  </si>
+  <si>
+    <t>Degree's Country of Origin</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Undergrad GPA</t>
+  </si>
+  <si>
+    <t>GRE General</t>
+  </si>
+  <si>
+    <t>GRE Verbal</t>
+  </si>
+  <si>
+    <t>Analytical Writing</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>985541</t>
+  </si>
+  <si>
+    <t>985521</t>
+  </si>
+  <si>
+    <t>985501</t>
+  </si>
+  <si>
+    <t>985481</t>
+  </si>
+  <si>
+    <t>985461</t>
+  </si>
+  <si>
+    <t>985441</t>
+  </si>
+  <si>
+    <t>985421</t>
   </si>
 </sst>
 </file>
@@ -380,23 +437,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>